<commit_message>
Updated rules and SCH
</commit_message>
<xml_diff>
--- a/rules/Reporting Requirements and Rules.xlsx
+++ b/rules/Reporting Requirements and Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\reporting\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD53439-F4FC-45EE-B51E-B0413093A879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A25D5F-6F8A-4F0F-BA3D-B618D311BFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{D55973C5-EE73-483F-94E6-D9DE17C4B093}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="258">
   <si>
     <t>ID</t>
   </si>
@@ -551,9 +551,6 @@
     <t>XSD only</t>
   </si>
   <si>
-    <t>Per Transport Protocol</t>
-  </si>
-  <si>
     <t>BR-TSR-01</t>
   </si>
   <si>
@@ -629,15 +626,6 @@
     <t>BR-TSR-25</t>
   </si>
   <si>
-    <t>Per SP; no longer explicit</t>
-  </si>
-  <si>
-    <t>Per Dataset Type; no longer explicit</t>
-  </si>
-  <si>
-    <t>Per Country to Country; no longer explicit</t>
-  </si>
-  <si>
     <t>Customization ID</t>
   </si>
   <si>
@@ -791,9 +779,6 @@
     <t>Each combination of Receiving Service Provider ID and Dataset Type ID, for which data is aggregated, MUST NOT occur more then once.</t>
   </si>
   <si>
-    <t>Removed</t>
-  </si>
-  <si>
     <t>Per SP and DT</t>
   </si>
   <si>
@@ -845,16 +830,19 @@
     <t>BR-TSR-34</t>
   </si>
   <si>
-    <t>BR-TSR-35</t>
-  </si>
-  <si>
-    <t>BR-TSR-36</t>
-  </si>
-  <si>
-    <t>BR-TSR-37</t>
-  </si>
-  <si>
-    <t>-- Rule was deleted</t>
+    <t>No explicit SCH rule</t>
+  </si>
+  <si>
+    <t>Per SP</t>
+  </si>
+  <si>
+    <t>Per DT</t>
+  </si>
+  <si>
+    <t>Per TP</t>
+  </si>
+  <si>
+    <t>Per CC</t>
   </si>
 </sst>
 </file>
@@ -901,7 +889,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,12 +905,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,7 +930,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -968,11 +950,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1799,7 +1776,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,7 +1784,7 @@
         <v>98</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1815,7 +1792,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>159</v>
@@ -1826,7 +1803,7 @@
         <v>100</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1834,7 +1811,7 @@
         <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1842,7 +1819,7 @@
         <v>102</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1850,7 +1827,7 @@
         <v>103</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,7 +1835,7 @@
         <v>104</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
         <v>159</v>
@@ -1869,7 +1846,7 @@
         <v>105</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1877,7 +1854,7 @@
         <v>106</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1885,7 +1862,7 @@
         <v>107</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,7 +1870,7 @@
         <v>108</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1901,7 +1878,7 @@
         <v>109</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1909,7 +1886,7 @@
         <v>110</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1917,7 +1894,7 @@
         <v>111</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1925,7 +1902,7 @@
         <v>112</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1933,7 +1910,7 @@
         <v>113</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1941,7 +1918,7 @@
         <v>114</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1949,7 +1926,7 @@
         <v>115</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1957,7 +1934,7 @@
         <v>116</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -1965,7 +1942,7 @@
         <v>117</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1973,7 +1950,7 @@
         <v>118</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1981,7 +1958,7 @@
         <v>119</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1989,7 +1966,7 @@
         <v>120</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2662,14 +2639,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB955338-4C1E-487A-8F9C-B3643191810A}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="85.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2683,40 +2663,40 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>159</v>
@@ -2724,57 +2704,57 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>159</v>
@@ -2782,13 +2762,13 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>159</v>
@@ -2796,316 +2776,304 @@
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>186</v>
+        <v>254</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>186</v>
+        <v>254</v>
+      </c>
+      <c r="D12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>172</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>174</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>175</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>187</v>
+        <v>255</v>
+      </c>
+      <c r="D16" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>206</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>240</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>179</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>160</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>180</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>181</v>
-      </c>
       <c r="B22" s="1" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>160</v>
+        <v>257</v>
+      </c>
+      <c r="D22" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>188</v>
+        <v>257</v>
+      </c>
+      <c r="D23" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>184</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>240</v>
+      <c r="B26" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>244</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>245</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>241</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>243</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>247</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>248</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>257</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>258</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>259</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>260</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>